<commit_message>
笔记：H5 node.js bootstrap vue angular react
</commit_message>
<xml_diff>
--- a/1做事八件套/总笔记整理表.xlsx
+++ b/1做事八件套/总笔记整理表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="104">
   <si>
     <t>内存</t>
   </si>
@@ -66,7 +66,7 @@
     <t>G硬盘</t>
   </si>
   <si>
-    <t>vue</t>
+    <t>vue 视频</t>
   </si>
   <si>
     <t>G:\本地磁盘D\陈运\新建文件夹\VUE</t>
@@ -282,13 +282,25 @@
     <t>培训电脑桌面截图</t>
   </si>
   <si>
-    <t>比较1</t>
+    <t>3 H5_bootrap_node</t>
+  </si>
+  <si>
+    <t>H5_bootrap_node笔记（待定：有个人记录）</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>笔记x.H5_bootrap_node</t>
   </si>
   <si>
     <t>H5_bootrap_node</t>
   </si>
   <si>
-    <t>H5_bootrap_node笔记（待定：有个人记录）</t>
+    <t>4 vue_angular_react</t>
+  </si>
+  <si>
+    <t>笔记3 vue未.docx</t>
   </si>
   <si>
     <t>web201802</t>
@@ -1012,7 +1024,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1054,6 +1066,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1409,12 +1424,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:XFD64"/>
+  <dimension ref="A1:XFD67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1948,13 +1963,13 @@
     <row r="40" customFormat="1" spans="1:10">
       <c r="A40" s="9"/>
       <c r="B40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
         <v>82</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="G40" s="14">
         <v>1</v>
@@ -1966,73 +1981,108 @@
     <row r="41" customFormat="1" spans="1:10">
       <c r="A41" s="9"/>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G41" s="5">
+      <c r="G41" s="15">
         <v>1</v>
       </c>
       <c r="J41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="42" customFormat="1" spans="1:7">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" customFormat="1" spans="1:10">
       <c r="A42" s="9"/>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
-      </c>
-      <c r="F42" t="s">
         <v>86</v>
       </c>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" customFormat="1" spans="1:7">
+      <c r="E42" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" customFormat="1" spans="1:10">
       <c r="A43" s="9"/>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1"/>
+      <c r="G43" s="5"/>
+      <c r="J43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" customFormat="1" spans="1:10">
+      <c r="A44" s="9"/>
+      <c r="B44"/>
+      <c r="D44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" customFormat="1" spans="1:7">
-      <c r="A44" s="9"/>
-      <c r="B44" t="s">
+      <c r="E44" s="1"/>
+      <c r="G44" s="5"/>
+      <c r="J44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" customFormat="1" spans="1:7">
+      <c r="A45" s="9"/>
+      <c r="B45" t="s">
         <v>26</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D45" t="s">
         <v>89</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="F45" t="s">
         <v>90</v>
       </c>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3" t="s">
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" customFormat="1" spans="1:7">
+      <c r="A46" s="9"/>
+      <c r="B46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="3"/>
+      <c r="E46" t="s">
+        <v>92</v>
+      </c>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" customFormat="1" spans="1:7">
+      <c r="A47" s="9"/>
+      <c r="B47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="3"/>
+      <c r="A48" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" s="3"/>
@@ -2081,13 +2131,22 @@
     </row>
     <row r="64" spans="1:1">
       <c r="A64" s="3"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="3"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="3"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:XFD2"/>
     <mergeCell ref="B3:L3"/>
-    <mergeCell ref="A4:A44"/>
-    <mergeCell ref="A45:A64"/>
+    <mergeCell ref="A4:A47"/>
+    <mergeCell ref="A48:A67"/>
     <mergeCell ref="C13:C20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2114,40 +2173,40 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>